<commit_message>
eliminei os row names dos outputs xlsx
</commit_message>
<xml_diff>
--- a/output/patologia_previa.xlsx
+++ b/output/patologia_previa.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
@@ -44,7 +44,22 @@
     <t>hipertensao_arterial</t>
   </si>
   <si>
+    <t>fib_auricular</t>
+  </si>
+  <si>
+    <t>pneumonia_comunidade</t>
+  </si>
+  <si>
+    <t>doenca_depressiva</t>
+  </si>
+  <si>
+    <t>hipotiroidismo</t>
+  </si>
+  <si>
     <t>nenhuma</t>
+  </si>
+  <si>
+    <t>tabagismo</t>
   </si>
   <si>
     <t>dislipidemia</t>
@@ -53,199 +68,19 @@
     <t>alcoolismo</t>
   </si>
   <si>
+    <t>doenca_cerebrovascular</t>
+  </si>
+  <si>
+    <t>doenca_ansiedade</t>
+  </si>
+  <si>
+    <t>insuf_venosa_periferica</t>
+  </si>
+  <si>
     <t>obesidade</t>
   </si>
   <si>
     <t>SAOS</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>74</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>77</t>
-  </si>
-  <si>
-    <t>79</t>
-  </si>
-  <si>
-    <t>82</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>92</t>
-  </si>
-  <si>
-    <t>93</t>
-  </si>
-  <si>
-    <t>94</t>
-  </si>
-  <si>
-    <t>99</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>109</t>
-  </si>
-  <si>
-    <t>113</t>
-  </si>
-  <si>
-    <t>115</t>
-  </si>
-  <si>
-    <t>119</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>125</t>
-  </si>
-  <si>
-    <t>126</t>
-  </si>
-  <si>
-    <t>128</t>
-  </si>
-  <si>
-    <t>134</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>136</t>
-  </si>
-  <si>
-    <t>137</t>
-  </si>
-  <si>
-    <t>138</t>
   </si>
 </sst>
 </file>
@@ -297,56 +132,79 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>15</v>
+      <c r="A2" t="n">
+        <v>1.0</v>
       </c>
       <c r="B2" t="n">
         <v>1.0</v>
@@ -358,7 +216,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F2" t="n">
         <v>0.0</v>
@@ -393,16 +251,37 @@
       <c r="P2" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>16</v>
+      <c r="A3" t="n">
+        <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D3" t="n">
         <v>1.0</v>
@@ -411,7 +290,7 @@
         <v>1.0</v>
       </c>
       <c r="F3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
@@ -443,13 +322,34 @@
       <c r="P3" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>17</v>
+      <c r="A4" t="n">
+        <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
@@ -461,10 +361,10 @@
         <v>0.0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G4" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H4" t="n">
         <v>0.0</v>
@@ -493,13 +393,34 @@
       <c r="P4" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>18</v>
+      <c r="A5" t="n">
+        <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="C5" t="n">
         <v>0.0</v>
@@ -514,10 +435,10 @@
         <v>0.0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H5" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I5" t="n">
         <v>0.0</v>
@@ -543,19 +464,40 @@
       <c r="P5" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>19</v>
+      <c r="A6" t="n">
+        <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D6" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E6" t="n">
         <v>0.0</v>
@@ -567,7 +509,7 @@
         <v>0.0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I6" t="n">
         <v>1.0</v>
@@ -576,7 +518,7 @@
         <v>1.0</v>
       </c>
       <c r="K6" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L6" t="n">
         <v>0.0</v>
@@ -593,43 +535,64 @@
       <c r="P6" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>20</v>
+      <c r="A7" t="n">
+        <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E7" t="n">
         <v>1.0</v>
       </c>
       <c r="F7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K7" t="n">
         <v>1.0</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M7" t="n">
         <v>0.0</v>
@@ -643,13 +606,34 @@
       <c r="P7" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>21</v>
+      <c r="A8" t="n">
+        <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
       <c r="C8" t="n">
         <v>0.0</v>
@@ -682,10 +666,10 @@
         <v>0.0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="O8" t="n">
         <v>0.0</v>
@@ -693,13 +677,34 @@
       <c r="P8" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>22</v>
+      <c r="A9" t="n">
+        <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="C9" t="n">
         <v>0.0</v>
@@ -729,7 +734,7 @@
         <v>0.0</v>
       </c>
       <c r="L9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M9" t="n">
         <v>0.0</v>
@@ -738,18 +743,39 @@
         <v>0.0</v>
       </c>
       <c r="O9" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P9" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>23</v>
+      <c r="A10" t="n">
+        <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="C10" t="n">
         <v>0.0</v>
@@ -758,25 +784,25 @@
         <v>0.0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G10" t="n">
         <v>0.0</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L10" t="n">
         <v>0.0</v>
@@ -791,15 +817,36 @@
         <v>0.0</v>
       </c>
       <c r="P10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W10" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>24</v>
+      <c r="A11" t="n">
+        <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="C11" t="n">
         <v>0.0</v>
@@ -832,7 +879,7 @@
         <v>0.0</v>
       </c>
       <c r="M11" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="N11" t="n">
         <v>0.0</v>
@@ -843,13 +890,34 @@
       <c r="P11" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>25</v>
+      <c r="A12" t="n">
+        <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c r="C12" t="n">
         <v>0.0</v>
@@ -885,7 +953,7 @@
         <v>0.0</v>
       </c>
       <c r="N12" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="O12" t="n">
         <v>0.0</v>
@@ -893,13 +961,34 @@
       <c r="P12" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>26</v>
+      <c r="A13" t="n">
+        <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="C13" t="n">
         <v>0.0</v>
@@ -923,10 +1012,10 @@
         <v>0.0</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K13" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L13" t="n">
         <v>0.0</v>
@@ -935,21 +1024,42 @@
         <v>0.0</v>
       </c>
       <c r="N13" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="O13" t="n">
         <v>0.0</v>
       </c>
       <c r="P13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W13" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>27</v>
+      <c r="A14" t="n">
+        <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
       <c r="C14" t="n">
         <v>0.0</v>
@@ -979,7 +1089,7 @@
         <v>0.0</v>
       </c>
       <c r="L14" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M14" t="n">
         <v>0.0</v>
@@ -988,18 +1098,39 @@
         <v>0.0</v>
       </c>
       <c r="O14" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P14" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>28</v>
+      <c r="A15" t="n">
+        <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
       <c r="C15" t="n">
         <v>0.0</v>
@@ -1029,7 +1160,7 @@
         <v>0.0</v>
       </c>
       <c r="L15" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M15" t="n">
         <v>0.0</v>
@@ -1038,18 +1169,39 @@
         <v>0.0</v>
       </c>
       <c r="O15" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P15" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W15" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>29</v>
+      <c r="A16" t="n">
+        <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="C16" t="n">
         <v>0.0</v>
@@ -1058,10 +1210,10 @@
         <v>0.0</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F16" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G16" t="n">
         <v>0.0</v>
@@ -1073,10 +1225,10 @@
         <v>0.0</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K16" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L16" t="n">
         <v>0.0</v>
@@ -1091,15 +1243,36 @@
         <v>0.0</v>
       </c>
       <c r="P16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W16" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>30</v>
+      <c r="A17" t="n">
+        <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>16.0</v>
+        <v>0.0</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
@@ -1123,16 +1296,16 @@
         <v>0.0</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K17" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L17" t="n">
         <v>0.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N17" t="n">
         <v>0.0</v>
@@ -1143,13 +1316,34 @@
       <c r="P17" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>31</v>
+      <c r="A18" t="n">
+        <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>17.0</v>
+        <v>0.0</v>
       </c>
       <c r="C18" t="n">
         <v>0.0</v>
@@ -1179,7 +1373,7 @@
         <v>0.0</v>
       </c>
       <c r="L18" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M18" t="n">
         <v>0.0</v>
@@ -1188,18 +1382,39 @@
         <v>0.0</v>
       </c>
       <c r="O18" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P18" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>32</v>
+      <c r="A19" t="n">
+        <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>18.0</v>
+        <v>0.0</v>
       </c>
       <c r="C19" t="n">
         <v>0.0</v>
@@ -1235,7 +1450,7 @@
         <v>0.0</v>
       </c>
       <c r="N19" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="O19" t="n">
         <v>0.0</v>
@@ -1243,25 +1458,46 @@
       <c r="P19" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W19" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>33</v>
+      <c r="A20" t="n">
+        <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>19.0</v>
+        <v>0.0</v>
       </c>
       <c r="C20" t="n">
         <v>0.0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E20" t="n">
         <v>1.0</v>
       </c>
       <c r="F20" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G20" t="n">
         <v>0.0</v>
@@ -1282,7 +1518,7 @@
         <v>0.0</v>
       </c>
       <c r="M20" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="N20" t="n">
         <v>0.0</v>
@@ -1291,27 +1527,48 @@
         <v>0.0</v>
       </c>
       <c r="P20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W20" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
-        <v>34</v>
+      <c r="A21" t="n">
+        <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D21" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F21" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G21" t="n">
         <v>0.0</v>
@@ -1320,10 +1577,10 @@
         <v>0.0</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J21" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K21" t="n">
         <v>0.0</v>
@@ -1341,15 +1598,36 @@
         <v>0.0</v>
       </c>
       <c r="P21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W21" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
-        <v>35</v>
+      <c r="A22" t="n">
+        <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>21.0</v>
+        <v>0.0</v>
       </c>
       <c r="C22" t="n">
         <v>0.0</v>
@@ -1373,16 +1651,16 @@
         <v>0.0</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K22" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L22" t="n">
         <v>0.0</v>
       </c>
       <c r="M22" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="N22" t="n">
         <v>0.0</v>
@@ -1393,34 +1671,55 @@
       <c r="P22" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W22" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
-        <v>36</v>
+      <c r="A23" t="n">
+        <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>22.0</v>
+        <v>0.0</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D23" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E23" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F23" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G23" t="n">
         <v>0.0</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I23" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J23" t="n">
         <v>0.0</v>
@@ -1435,7 +1734,7 @@
         <v>0.0</v>
       </c>
       <c r="N23" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="O23" t="n">
         <v>0.0</v>
@@ -1443,13 +1742,34 @@
       <c r="P23" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W23" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" t="s">
-        <v>37</v>
+      <c r="A24" t="n">
+        <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>23.0</v>
+        <v>0.0</v>
       </c>
       <c r="C24" t="n">
         <v>0.0</v>
@@ -1482,7 +1802,7 @@
         <v>0.0</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N24" t="n">
         <v>0.0</v>
@@ -1493,13 +1813,34 @@
       <c r="P24" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" t="s">
-        <v>38</v>
+      <c r="A25" t="n">
+        <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="C25" t="n">
         <v>0.0</v>
@@ -1529,7 +1870,7 @@
         <v>0.0</v>
       </c>
       <c r="L25" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M25" t="n">
         <v>0.0</v>
@@ -1538,18 +1879,39 @@
         <v>0.0</v>
       </c>
       <c r="O25" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P25" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
-        <v>39</v>
+      <c r="A26" t="n">
+        <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>25.0</v>
+        <v>0.0</v>
       </c>
       <c r="C26" t="n">
         <v>0.0</v>
@@ -1558,10 +1920,10 @@
         <v>0.0</v>
       </c>
       <c r="E26" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F26" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G26" t="n">
         <v>0.0</v>
@@ -1591,15 +1953,36 @@
         <v>0.0</v>
       </c>
       <c r="P26" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U26" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W26" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s">
-        <v>40</v>
+      <c r="A27" t="n">
+        <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>26.0</v>
+        <v>0.0</v>
       </c>
       <c r="C27" t="n">
         <v>0.0</v>
@@ -1643,13 +2026,34 @@
       <c r="P27" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" t="s">
-        <v>41</v>
+      <c r="A28" t="n">
+        <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>27.0</v>
+        <v>0.0</v>
       </c>
       <c r="C28" t="n">
         <v>0.0</v>
@@ -1679,7 +2083,7 @@
         <v>0.0</v>
       </c>
       <c r="L28" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M28" t="n">
         <v>0.0</v>
@@ -1688,24 +2092,45 @@
         <v>0.0</v>
       </c>
       <c r="O28" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P28" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="s">
-        <v>42</v>
+      <c r="A29" t="n">
+        <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>28.0</v>
+        <v>0.0</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D29" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E29" t="n">
         <v>0.0</v>
@@ -1743,13 +2168,34 @@
       <c r="P29" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" t="s">
-        <v>43</v>
+      <c r="A30" t="n">
+        <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>29.0</v>
+        <v>0.0</v>
       </c>
       <c r="C30" t="n">
         <v>0.0</v>
@@ -1779,7 +2225,7 @@
         <v>0.0</v>
       </c>
       <c r="L30" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M30" t="n">
         <v>0.0</v>
@@ -1788,18 +2234,39 @@
         <v>0.0</v>
       </c>
       <c r="O30" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P30" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
-        <v>44</v>
+      <c r="A31" t="n">
+        <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>30.0</v>
+        <v>0.0</v>
       </c>
       <c r="C31" t="n">
         <v>0.0</v>
@@ -1829,7 +2296,7 @@
         <v>0.0</v>
       </c>
       <c r="L31" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M31" t="n">
         <v>0.0</v>
@@ -1838,24 +2305,45 @@
         <v>0.0</v>
       </c>
       <c r="O31" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P31" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
-        <v>45</v>
+      <c r="A32" t="n">
+        <v>31.0</v>
       </c>
       <c r="B32" t="n">
-        <v>31.0</v>
+        <v>0.0</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D32" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E32" t="n">
         <v>0.0</v>
@@ -1885,21 +2373,42 @@
         <v>0.0</v>
       </c>
       <c r="N32" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="O32" t="n">
         <v>0.0</v>
       </c>
       <c r="P32" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R32" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W32" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
-        <v>46</v>
+      <c r="A33" t="n">
+        <v>32.0</v>
       </c>
       <c r="B33" t="n">
-        <v>32.0</v>
+        <v>0.0</v>
       </c>
       <c r="C33" t="n">
         <v>0.0</v>
@@ -1923,10 +2432,10 @@
         <v>0.0</v>
       </c>
       <c r="J33" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K33" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L33" t="n">
         <v>0.0</v>
@@ -1943,13 +2452,34 @@
       <c r="P33" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" t="s">
-        <v>47</v>
+      <c r="A34" t="n">
+        <v>33.0</v>
       </c>
       <c r="B34" t="n">
-        <v>33.0</v>
+        <v>0.0</v>
       </c>
       <c r="C34" t="n">
         <v>0.0</v>
@@ -1993,13 +2523,34 @@
       <c r="P34" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" t="s">
-        <v>48</v>
+      <c r="A35" t="n">
+        <v>34.0</v>
       </c>
       <c r="B35" t="n">
-        <v>34.0</v>
+        <v>0.0</v>
       </c>
       <c r="C35" t="n">
         <v>0.0</v>
@@ -2029,7 +2580,7 @@
         <v>0.0</v>
       </c>
       <c r="L35" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M35" t="n">
         <v>0.0</v>
@@ -2038,18 +2589,39 @@
         <v>0.0</v>
       </c>
       <c r="O35" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P35" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" t="s">
-        <v>49</v>
+      <c r="A36" t="n">
+        <v>35.0</v>
       </c>
       <c r="B36" t="n">
-        <v>35.0</v>
+        <v>0.0</v>
       </c>
       <c r="C36" t="n">
         <v>0.0</v>
@@ -2082,24 +2654,45 @@
         <v>0.0</v>
       </c>
       <c r="M36" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="N36" t="n">
         <v>0.0</v>
       </c>
       <c r="O36" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P36" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q36" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V36" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W36" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" t="s">
-        <v>50</v>
+      <c r="A37" t="n">
+        <v>36.0</v>
       </c>
       <c r="B37" t="n">
-        <v>36.0</v>
+        <v>0.0</v>
       </c>
       <c r="C37" t="n">
         <v>0.0</v>
@@ -2138,18 +2731,39 @@
         <v>0.0</v>
       </c>
       <c r="O37" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P37" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V37" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W37" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
-        <v>51</v>
+      <c r="A38" t="n">
+        <v>37.0</v>
       </c>
       <c r="B38" t="n">
-        <v>37.0</v>
+        <v>0.0</v>
       </c>
       <c r="C38" t="n">
         <v>0.0</v>
@@ -2158,10 +2772,10 @@
         <v>0.0</v>
       </c>
       <c r="E38" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F38" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G38" t="n">
         <v>0.0</v>
@@ -2173,10 +2787,10 @@
         <v>0.0</v>
       </c>
       <c r="J38" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K38" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L38" t="n">
         <v>0.0</v>
@@ -2191,18 +2805,39 @@
         <v>0.0</v>
       </c>
       <c r="P38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W38" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s">
-        <v>52</v>
+      <c r="A39" t="n">
+        <v>38.0</v>
       </c>
       <c r="B39" t="n">
-        <v>38.0</v>
+        <v>0.0</v>
       </c>
       <c r="C39" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D39" t="n">
         <v>1.0</v>
@@ -2211,45 +2846,66 @@
         <v>1.0</v>
       </c>
       <c r="F39" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G39" t="n">
         <v>0.0</v>
       </c>
       <c r="H39" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I39" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J39" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K39" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L39" t="n">
         <v>0.0</v>
       </c>
       <c r="M39" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="N39" t="n">
         <v>0.0</v>
       </c>
       <c r="O39" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P39" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q39" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V39" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W39" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" t="s">
-        <v>53</v>
+      <c r="A40" t="n">
+        <v>39.0</v>
       </c>
       <c r="B40" t="n">
-        <v>39.0</v>
+        <v>0.0</v>
       </c>
       <c r="C40" t="n">
         <v>0.0</v>
@@ -2285,7 +2941,7 @@
         <v>0.0</v>
       </c>
       <c r="N40" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="O40" t="n">
         <v>0.0</v>
@@ -2293,13 +2949,34 @@
       <c r="P40" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R40" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W40" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" t="s">
-        <v>54</v>
+      <c r="A41" t="n">
+        <v>40.0</v>
       </c>
       <c r="B41" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="C41" t="n">
         <v>0.0</v>
@@ -2329,7 +3006,7 @@
         <v>0.0</v>
       </c>
       <c r="L41" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M41" t="n">
         <v>0.0</v>
@@ -2338,18 +3015,39 @@
         <v>0.0</v>
       </c>
       <c r="O41" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P41" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W41" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" t="s">
-        <v>55</v>
+      <c r="A42" t="n">
+        <v>41.0</v>
       </c>
       <c r="B42" t="n">
-        <v>41.0</v>
+        <v>0.0</v>
       </c>
       <c r="C42" t="n">
         <v>0.0</v>
@@ -2393,25 +3091,46 @@
       <c r="P42" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q42" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R42" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T42" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U42" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V42" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W42" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" t="s">
-        <v>56</v>
+      <c r="A43" t="n">
+        <v>42.0</v>
       </c>
       <c r="B43" t="n">
-        <v>42.0</v>
+        <v>0.0</v>
       </c>
       <c r="C43" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D43" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E43" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F43" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G43" t="n">
         <v>0.0</v>
@@ -2432,24 +3151,45 @@
         <v>0.0</v>
       </c>
       <c r="M43" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="N43" t="n">
         <v>0.0</v>
       </c>
       <c r="O43" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P43" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q43" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V43" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W43" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" t="s">
-        <v>57</v>
+      <c r="A44" t="n">
+        <v>43.0</v>
       </c>
       <c r="B44" t="n">
-        <v>43.0</v>
+        <v>0.0</v>
       </c>
       <c r="C44" t="n">
         <v>0.0</v>
@@ -2482,7 +3222,7 @@
         <v>0.0</v>
       </c>
       <c r="M44" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N44" t="n">
         <v>0.0</v>
@@ -2493,13 +3233,34 @@
       <c r="P44" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W44" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" t="s">
-        <v>58</v>
+      <c r="A45" t="n">
+        <v>44.0</v>
       </c>
       <c r="B45" t="n">
-        <v>44.0</v>
+        <v>0.0</v>
       </c>
       <c r="C45" t="n">
         <v>0.0</v>
@@ -2529,7 +3290,7 @@
         <v>0.0</v>
       </c>
       <c r="L45" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M45" t="n">
         <v>0.0</v>
@@ -2538,18 +3299,39 @@
         <v>0.0</v>
       </c>
       <c r="O45" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P45" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q45" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R45" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S45" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T45" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U45" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V45" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W45" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" t="s">
-        <v>59</v>
+      <c r="A46" t="n">
+        <v>45.0</v>
       </c>
       <c r="B46" t="n">
-        <v>45.0</v>
+        <v>0.0</v>
       </c>
       <c r="C46" t="n">
         <v>0.0</v>
@@ -2593,13 +3375,34 @@
       <c r="P46" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V46" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W46" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" t="s">
-        <v>60</v>
+      <c r="A47" t="n">
+        <v>46.0</v>
       </c>
       <c r="B47" t="n">
-        <v>46.0</v>
+        <v>0.0</v>
       </c>
       <c r="C47" t="n">
         <v>0.0</v>
@@ -2632,7 +3435,7 @@
         <v>0.0</v>
       </c>
       <c r="M47" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="N47" t="n">
         <v>0.0</v>
@@ -2643,40 +3446,61 @@
       <c r="P47" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q47" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V47" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W47" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" t="s">
-        <v>61</v>
+      <c r="A48" t="n">
+        <v>47.0</v>
       </c>
       <c r="B48" t="n">
-        <v>47.0</v>
+        <v>1.0</v>
       </c>
       <c r="C48" t="n">
         <v>1.0</v>
       </c>
       <c r="D48" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E48" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F48" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G48" t="n">
         <v>0.0</v>
       </c>
       <c r="H48" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I48" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J48" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K48" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L48" t="n">
         <v>0.0</v>
@@ -2693,19 +3517,40 @@
       <c r="P48" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V48" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W48" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" t="s">
-        <v>62</v>
+      <c r="A49" t="n">
+        <v>48.0</v>
       </c>
       <c r="B49" t="n">
-        <v>48.0</v>
+        <v>0.0</v>
       </c>
       <c r="C49" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D49" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E49" t="n">
         <v>0.0</v>
@@ -2717,19 +3562,19 @@
         <v>0.0</v>
       </c>
       <c r="H49" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I49" t="n">
         <v>1.0</v>
       </c>
       <c r="J49" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K49" t="n">
         <v>0.0</v>
       </c>
       <c r="L49" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M49" t="n">
         <v>0.0</v>
@@ -2743,13 +3588,34 @@
       <c r="P49" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V49" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W49" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" t="s">
-        <v>63</v>
+      <c r="A50" t="n">
+        <v>49.0</v>
       </c>
       <c r="B50" t="n">
-        <v>49.0</v>
+        <v>0.0</v>
       </c>
       <c r="C50" t="n">
         <v>0.0</v>
@@ -2782,45 +3648,66 @@
         <v>0.0</v>
       </c>
       <c r="M50" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="N50" t="n">
         <v>0.0</v>
       </c>
       <c r="O50" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P50" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W50" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" t="s">
-        <v>64</v>
+      <c r="A51" t="n">
+        <v>50.0</v>
       </c>
       <c r="B51" t="n">
-        <v>50.0</v>
+        <v>1.0</v>
       </c>
       <c r="C51" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D51" t="n">
         <v>0.0</v>
       </c>
       <c r="E51" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F51" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G51" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H51" t="n">
         <v>1.0</v>
       </c>
       <c r="I51" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J51" t="n">
         <v>0.0</v>
@@ -2843,13 +3730,34 @@
       <c r="P51" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W51" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" t="s">
-        <v>65</v>
+      <c r="A52" t="n">
+        <v>51.0</v>
       </c>
       <c r="B52" t="n">
-        <v>51.0</v>
+        <v>0.0</v>
       </c>
       <c r="C52" t="n">
         <v>0.0</v>
@@ -2888,18 +3796,39 @@
         <v>0.0</v>
       </c>
       <c r="O52" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P52" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q52" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R52" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S52" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T52" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U52" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V52" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W52" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" t="s">
-        <v>66</v>
+      <c r="A53" t="n">
+        <v>52.0</v>
       </c>
       <c r="B53" t="n">
-        <v>52.0</v>
+        <v>0.0</v>
       </c>
       <c r="C53" t="n">
         <v>0.0</v>
@@ -2914,13 +3843,13 @@
         <v>0.0</v>
       </c>
       <c r="G53" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H53" t="n">
         <v>1.0</v>
       </c>
       <c r="I53" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J53" t="n">
         <v>0.0</v>
@@ -2943,13 +3872,34 @@
       <c r="P53" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V53" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W53" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" t="s">
-        <v>67</v>
+      <c r="A54" t="n">
+        <v>53.0</v>
       </c>
       <c r="B54" t="n">
-        <v>53.0</v>
+        <v>0.0</v>
       </c>
       <c r="C54" t="n">
         <v>0.0</v>
@@ -2979,7 +3929,7 @@
         <v>0.0</v>
       </c>
       <c r="L54" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M54" t="n">
         <v>0.0</v>
@@ -2988,18 +3938,39 @@
         <v>0.0</v>
       </c>
       <c r="O54" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P54" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q54" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R54" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S54" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T54" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U54" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V54" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W54" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" t="s">
-        <v>68</v>
+      <c r="A55" t="n">
+        <v>54.0</v>
       </c>
       <c r="B55" t="n">
-        <v>54.0</v>
+        <v>0.0</v>
       </c>
       <c r="C55" t="n">
         <v>0.0</v>
@@ -3029,7 +4000,7 @@
         <v>0.0</v>
       </c>
       <c r="L55" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M55" t="n">
         <v>0.0</v>
@@ -3038,18 +4009,39 @@
         <v>0.0</v>
       </c>
       <c r="O55" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P55" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V55" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W55" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" t="s">
-        <v>69</v>
+      <c r="A56" t="n">
+        <v>55.0</v>
       </c>
       <c r="B56" t="n">
-        <v>55.0</v>
+        <v>0.0</v>
       </c>
       <c r="C56" t="n">
         <v>0.0</v>
@@ -3079,7 +4071,7 @@
         <v>0.0</v>
       </c>
       <c r="L56" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M56" t="n">
         <v>0.0</v>
@@ -3088,18 +4080,39 @@
         <v>0.0</v>
       </c>
       <c r="O56" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P56" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W56" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" t="s">
-        <v>70</v>
+      <c r="A57" t="n">
+        <v>56.0</v>
       </c>
       <c r="B57" t="n">
-        <v>56.0</v>
+        <v>0.0</v>
       </c>
       <c r="C57" t="n">
         <v>0.0</v>
@@ -3129,7 +4142,7 @@
         <v>0.0</v>
       </c>
       <c r="L57" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M57" t="n">
         <v>0.0</v>
@@ -3138,18 +4151,39 @@
         <v>0.0</v>
       </c>
       <c r="O57" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P57" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W57" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" t="s">
-        <v>71</v>
+      <c r="A58" t="n">
+        <v>57.0</v>
       </c>
       <c r="B58" t="n">
-        <v>57.0</v>
+        <v>0.0</v>
       </c>
       <c r="C58" t="n">
         <v>0.0</v>
@@ -3164,13 +4198,13 @@
         <v>0.0</v>
       </c>
       <c r="G58" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H58" t="n">
         <v>1.0</v>
       </c>
       <c r="I58" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J58" t="n">
         <v>0.0</v>
@@ -3193,16 +4227,37 @@
       <c r="P58" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W58" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" t="s">
-        <v>72</v>
+      <c r="A59" t="n">
+        <v>58.0</v>
       </c>
       <c r="B59" t="n">
-        <v>58.0</v>
+        <v>0.0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D59" t="n">
         <v>1.0</v>
@@ -3211,16 +4266,16 @@
         <v>1.0</v>
       </c>
       <c r="F59" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G59" t="n">
         <v>0.0</v>
       </c>
       <c r="H59" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I59" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J59" t="n">
         <v>0.0</v>
@@ -3232,24 +4287,45 @@
         <v>0.0</v>
       </c>
       <c r="M59" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="N59" t="n">
         <v>0.0</v>
       </c>
       <c r="O59" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P59" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q59" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V59" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W59" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" t="s">
-        <v>73</v>
+      <c r="A60" t="n">
+        <v>59.0</v>
       </c>
       <c r="B60" t="n">
-        <v>59.0</v>
+        <v>0.0</v>
       </c>
       <c r="C60" t="n">
         <v>0.0</v>
@@ -3279,7 +4355,7 @@
         <v>0.0</v>
       </c>
       <c r="L60" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M60" t="n">
         <v>0.0</v>
@@ -3288,18 +4364,39 @@
         <v>0.0</v>
       </c>
       <c r="O60" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P60" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W60" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" t="s">
-        <v>74</v>
+      <c r="A61" t="n">
+        <v>60.0</v>
       </c>
       <c r="B61" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
       <c r="C61" t="n">
         <v>0.0</v>
@@ -3329,7 +4426,7 @@
         <v>0.0</v>
       </c>
       <c r="L61" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M61" t="n">
         <v>0.0</v>
@@ -3338,18 +4435,39 @@
         <v>0.0</v>
       </c>
       <c r="O61" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P61" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q61" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R61" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S61" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T61" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U61" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V61" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W61" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" t="s">
-        <v>75</v>
+      <c r="A62" t="n">
+        <v>61.0</v>
       </c>
       <c r="B62" t="n">
-        <v>61.0</v>
+        <v>0.0</v>
       </c>
       <c r="C62" t="n">
         <v>0.0</v>
@@ -3385,7 +4503,7 @@
         <v>0.0</v>
       </c>
       <c r="N62" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="O62" t="n">
         <v>0.0</v>
@@ -3393,13 +4511,34 @@
       <c r="P62" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q62" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R62" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S62" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T62" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U62" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V62" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W62" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" t="s">
-        <v>76</v>
+      <c r="A63" t="n">
+        <v>62.0</v>
       </c>
       <c r="B63" t="n">
-        <v>62.0</v>
+        <v>0.0</v>
       </c>
       <c r="C63" t="n">
         <v>0.0</v>
@@ -3429,7 +4568,7 @@
         <v>0.0</v>
       </c>
       <c r="L63" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M63" t="n">
         <v>0.0</v>
@@ -3438,18 +4577,39 @@
         <v>0.0</v>
       </c>
       <c r="O63" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P63" t="n">
         <v>0.0</v>
       </c>
+      <c r="Q63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V63" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W63" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" t="s">
-        <v>77</v>
+      <c r="A64" t="n">
+        <v>63.0</v>
       </c>
       <c r="B64" t="n">
-        <v>63.0</v>
+        <v>0.0</v>
       </c>
       <c r="C64" t="n">
         <v>0.0</v>
@@ -3458,10 +4618,10 @@
         <v>0.0</v>
       </c>
       <c r="E64" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F64" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G64" t="n">
         <v>0.0</v>
@@ -3488,9 +4648,30 @@
         <v>0.0</v>
       </c>
       <c r="O64" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="P64" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q64" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R64" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S64" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="T64" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U64" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V64" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W64" t="n">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corrigiu o erro ao tentar tirar o row names do principal.xlsx
</commit_message>
<xml_diff>
--- a/output/patologia_previa.xlsx
+++ b/output/patologia_previa.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>doenca_ansiedade</t>
+  </si>
+  <si>
+    <t>doenca_renal_cronica</t>
   </si>
   <si>
     <t>insuf_venosa_periferica</t>
@@ -201,6 +204,9 @@
       <c r="W1" t="s">
         <v>22</v>
       </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -270,6 +276,9 @@
         <v>0.0</v>
       </c>
       <c r="W2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X2" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -343,6 +352,9 @@
       <c r="W3" t="n">
         <v>0.0</v>
       </c>
+      <c r="X3" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -414,6 +426,9 @@
       <c r="W4" t="n">
         <v>0.0</v>
       </c>
+      <c r="X4" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -485,6 +500,9 @@
       <c r="W5" t="n">
         <v>0.0</v>
       </c>
+      <c r="X5" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -556,6 +574,9 @@
       <c r="W6" t="n">
         <v>0.0</v>
       </c>
+      <c r="X6" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -627,6 +648,9 @@
       <c r="W7" t="n">
         <v>0.0</v>
       </c>
+      <c r="X7" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -698,6 +722,9 @@
       <c r="W8" t="n">
         <v>0.0</v>
       </c>
+      <c r="X8" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -769,6 +796,9 @@
       <c r="W9" t="n">
         <v>0.0</v>
       </c>
+      <c r="X9" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -840,6 +870,9 @@
       <c r="W10" t="n">
         <v>0.0</v>
       </c>
+      <c r="X10" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -911,6 +944,9 @@
       <c r="W11" t="n">
         <v>0.0</v>
       </c>
+      <c r="X11" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -982,6 +1018,9 @@
       <c r="W12" t="n">
         <v>0.0</v>
       </c>
+      <c r="X12" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1053,6 +1092,9 @@
       <c r="W13" t="n">
         <v>0.0</v>
       </c>
+      <c r="X13" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1124,6 +1166,9 @@
       <c r="W14" t="n">
         <v>0.0</v>
       </c>
+      <c r="X14" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1195,6 +1240,9 @@
       <c r="W15" t="n">
         <v>0.0</v>
       </c>
+      <c r="X15" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1266,6 +1314,9 @@
       <c r="W16" t="n">
         <v>0.0</v>
       </c>
+      <c r="X16" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1337,6 +1388,9 @@
       <c r="W17" t="n">
         <v>0.0</v>
       </c>
+      <c r="X17" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1408,6 +1462,9 @@
       <c r="W18" t="n">
         <v>0.0</v>
       </c>
+      <c r="X18" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1479,6 +1536,9 @@
       <c r="W19" t="n">
         <v>0.0</v>
       </c>
+      <c r="X19" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1550,6 +1610,9 @@
       <c r="W20" t="n">
         <v>0.0</v>
       </c>
+      <c r="X20" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1621,6 +1684,9 @@
       <c r="W21" t="n">
         <v>0.0</v>
       </c>
+      <c r="X21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1692,6 +1758,9 @@
       <c r="W22" t="n">
         <v>0.0</v>
       </c>
+      <c r="X22" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1755,12 +1824,15 @@
         <v>0.0</v>
       </c>
       <c r="U23" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V23" t="n">
         <v>0.0</v>
       </c>
       <c r="W23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X23" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -1834,6 +1906,9 @@
       <c r="W24" t="n">
         <v>0.0</v>
       </c>
+      <c r="X24" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1905,6 +1980,9 @@
       <c r="W25" t="n">
         <v>0.0</v>
       </c>
+      <c r="X25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1968,12 +2046,15 @@
         <v>0.0</v>
       </c>
       <c r="U26" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="V26" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="W26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X26" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2047,6 +2128,9 @@
       <c r="W27" t="n">
         <v>0.0</v>
       </c>
+      <c r="X27" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2118,6 +2202,9 @@
       <c r="W28" t="n">
         <v>0.0</v>
       </c>
+      <c r="X28" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2189,6 +2276,9 @@
       <c r="W29" t="n">
         <v>0.0</v>
       </c>
+      <c r="X29" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2260,6 +2350,9 @@
       <c r="W30" t="n">
         <v>0.0</v>
       </c>
+      <c r="X30" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2331,6 +2424,9 @@
       <c r="W31" t="n">
         <v>0.0</v>
       </c>
+      <c r="X31" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2402,6 +2498,9 @@
       <c r="W32" t="n">
         <v>0.0</v>
       </c>
+      <c r="X32" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2473,6 +2572,9 @@
       <c r="W33" t="n">
         <v>0.0</v>
       </c>
+      <c r="X33" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2544,6 +2646,9 @@
       <c r="W34" t="n">
         <v>0.0</v>
       </c>
+      <c r="X34" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2615,6 +2720,9 @@
       <c r="W35" t="n">
         <v>0.0</v>
       </c>
+      <c r="X35" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2681,9 +2789,12 @@
         <v>0.0</v>
       </c>
       <c r="V36" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W36" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X36" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2752,9 +2863,12 @@
         <v>0.0</v>
       </c>
       <c r="V37" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W37" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X37" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2826,6 +2940,9 @@
         <v>0.0</v>
       </c>
       <c r="W38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X38" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -2894,9 +3011,12 @@
         <v>0.0</v>
       </c>
       <c r="V39" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W39" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X39" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2970,6 +3090,9 @@
       <c r="W40" t="n">
         <v>0.0</v>
       </c>
+      <c r="X40" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -3041,6 +3164,9 @@
       <c r="W41" t="n">
         <v>0.0</v>
       </c>
+      <c r="X41" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -3112,6 +3238,9 @@
       <c r="W42" t="n">
         <v>0.0</v>
       </c>
+      <c r="X42" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -3178,9 +3307,12 @@
         <v>0.0</v>
       </c>
       <c r="V43" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W43" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X43" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -3254,6 +3386,9 @@
       <c r="W44" t="n">
         <v>0.0</v>
       </c>
+      <c r="X44" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3325,6 +3460,9 @@
       <c r="W45" t="n">
         <v>0.0</v>
       </c>
+      <c r="X45" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -3396,6 +3534,9 @@
       <c r="W46" t="n">
         <v>0.0</v>
       </c>
+      <c r="X46" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -3467,6 +3608,9 @@
       <c r="W47" t="n">
         <v>0.0</v>
       </c>
+      <c r="X47" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -3538,6 +3682,9 @@
       <c r="W48" t="n">
         <v>0.0</v>
       </c>
+      <c r="X48" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -3609,6 +3756,9 @@
       <c r="W49" t="n">
         <v>0.0</v>
       </c>
+      <c r="X49" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -3675,9 +3825,12 @@
         <v>0.0</v>
       </c>
       <c r="V50" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W50" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X50" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -3751,6 +3904,9 @@
       <c r="W51" t="n">
         <v>0.0</v>
       </c>
+      <c r="X51" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3817,9 +3973,12 @@
         <v>0.0</v>
       </c>
       <c r="V52" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W52" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X52" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -3893,6 +4052,9 @@
       <c r="W53" t="n">
         <v>0.0</v>
       </c>
+      <c r="X53" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -3964,6 +4126,9 @@
       <c r="W54" t="n">
         <v>0.0</v>
       </c>
+      <c r="X54" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -4035,6 +4200,9 @@
       <c r="W55" t="n">
         <v>0.0</v>
       </c>
+      <c r="X55" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -4106,6 +4274,9 @@
       <c r="W56" t="n">
         <v>0.0</v>
       </c>
+      <c r="X56" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -4177,6 +4348,9 @@
       <c r="W57" t="n">
         <v>0.0</v>
       </c>
+      <c r="X57" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -4248,6 +4422,9 @@
       <c r="W58" t="n">
         <v>0.0</v>
       </c>
+      <c r="X58" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -4314,9 +4491,12 @@
         <v>0.0</v>
       </c>
       <c r="V59" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W59" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X59" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -4390,6 +4570,9 @@
       <c r="W60" t="n">
         <v>0.0</v>
       </c>
+      <c r="X60" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -4461,6 +4644,9 @@
       <c r="W61" t="n">
         <v>0.0</v>
       </c>
+      <c r="X61" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -4532,6 +4718,9 @@
       <c r="W62" t="n">
         <v>0.0</v>
       </c>
+      <c r="X62" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -4603,6 +4792,9 @@
       <c r="W63" t="n">
         <v>0.0</v>
       </c>
+      <c r="X63" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -4669,9 +4861,12 @@
         <v>0.0</v>
       </c>
       <c r="V64" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="W64" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X64" t="n">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>